<commit_message>
09.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/October/Others/SP Target Oct'2020 - Rajshahi.xlsx
+++ b/2020/October/Others/SP Target Oct'2020 - Rajshahi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BM Modality_EO" sheetId="2" r:id="rId1"/>
@@ -3312,8 +3312,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B2:N2149"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E232" sqref="E232:N317"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J190" sqref="J190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -41838,7 +41838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9:J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>